<commit_message>
Added KTM Komuter Routes
</commit_message>
<xml_diff>
--- a/Dataset/KTM Komuter.xlsx
+++ b/Dataset/KTM Komuter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JasonX\PycharmProjects\Algo-Assignment\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{909DBE2E-D36C-49FF-B403-42D9D0A63B7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA02EB20-577F-4D0D-8E83-DC32F4DC4DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3DFF64DC-D989-47BF-B042-34AAD9B60226}"/>
   </bookViews>
@@ -916,7 +916,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>